<commit_message>
bug fixes and peewee orm changed to sqlalchemy
</commit_message>
<xml_diff>
--- a/room_322.xlsx
+++ b/room_322.xlsx
@@ -502,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1209,7 +1209,7 @@
       <c r="I25" s="9" t="n"/>
       <c r="J25" s="12" t="inlineStr">
         <is>
-          <t>4051, 4052</t>
+          <t>4051</t>
         </is>
       </c>
       <c r="K25" s="9" t="n"/>
@@ -1229,277 +1229,242 @@
       <c r="K26" s="16" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
+      <c r="J27" s="6" t="inlineStr">
+        <is>
+          <t>ЛАБОРАТОРНАЯ</t>
+        </is>
+      </c>
+      <c r="K27" s="7" t="inlineStr">
+        <is>
+          <t>З</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="J28" s="11" t="n"/>
+      <c r="K28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="100" customHeight="1">
+      <c r="J29" s="14" t="inlineStr">
+        <is>
+          <t>Физико-химические основы технологии электроники и наноэлектр</t>
+        </is>
+      </c>
+      <c r="K29" s="9" t="n"/>
+    </row>
+    <row r="30">
+      <c r="J30" s="11" t="inlineStr">
+        <is>
+          <t>Короневский Н. В.</t>
+        </is>
+      </c>
+      <c r="K30" s="9" t="n"/>
+    </row>
+    <row r="31" ht="30" customHeight="1">
+      <c r="J31" s="14" t="inlineStr">
+        <is>
+          <t>4052</t>
+        </is>
+      </c>
+      <c r="K31" s="9" t="n"/>
+    </row>
+    <row r="32">
+      <c r="J32" s="18" t="inlineStr">
+        <is>
+          <t>8 корп. ауд. 322</t>
+        </is>
+      </c>
+      <c r="K32" s="16" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
         <is>
           <t>13:50 - 15:25</t>
         </is>
       </c>
-      <c r="B27" s="4" t="inlineStr">
+      <c r="B33" s="4" t="inlineStr">
         <is>
           <t>ЛЕКЦИЯ</t>
         </is>
       </c>
-      <c r="C27" s="5" t="inlineStr">
+      <c r="C33" s="5" t="inlineStr">
         <is>
           <t>Ч</t>
         </is>
       </c>
-      <c r="D27" s="6" t="inlineStr">
+      <c r="D33" s="6" t="inlineStr">
         <is>
           <t>ЛАБОРАТОРНАЯ</t>
         </is>
       </c>
-      <c r="E27" s="7" t="inlineStr">
+      <c r="E33" s="7" t="inlineStr">
         <is>
           <t>Ч/З</t>
         </is>
       </c>
-      <c r="F27" s="2" t="inlineStr">
+      <c r="F33" s="2" t="inlineStr">
         <is>
           <t>ПРАКТИКА</t>
         </is>
       </c>
-      <c r="G27" s="3" t="inlineStr">
+      <c r="G33" s="3" t="inlineStr">
         <is>
           <t>Ч/З</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="B28" s="10" t="n"/>
-      <c r="C28" s="9" t="n"/>
-      <c r="D28" s="11" t="n"/>
-      <c r="E28" s="9" t="n"/>
-      <c r="F28" s="8" t="n"/>
-      <c r="G28" s="9" t="n"/>
-    </row>
-    <row r="29" ht="100" customHeight="1">
-      <c r="B29" s="13" t="inlineStr">
+    <row r="34">
+      <c r="B34" s="10" t="n"/>
+      <c r="C34" s="9" t="n"/>
+      <c r="D34" s="11" t="n"/>
+      <c r="E34" s="9" t="n"/>
+      <c r="F34" s="8" t="n"/>
+      <c r="G34" s="9" t="n"/>
+    </row>
+    <row r="35" ht="100" customHeight="1">
+      <c r="B35" s="13" t="inlineStr">
         <is>
           <t>Молекулярные технологии и электроника</t>
         </is>
       </c>
-      <c r="C29" s="9" t="n"/>
-      <c r="D29" s="14" t="inlineStr">
+      <c r="C35" s="9" t="n"/>
+      <c r="D35" s="14" t="inlineStr">
         <is>
           <t>Методы измерений и испытаний полупроводниковых структур электроники</t>
         </is>
       </c>
-      <c r="E29" s="9" t="n"/>
-      <c r="F29" s="12" t="inlineStr">
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="12" t="inlineStr">
         <is>
           <t>Компьютерные технологии в научных исследованиях</t>
         </is>
       </c>
-      <c r="G29" s="9" t="n"/>
-    </row>
-    <row r="30">
-      <c r="B30" s="10" t="inlineStr">
+      <c r="G35" s="9" t="n"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="10" t="inlineStr">
         <is>
           <t>Ушаков Н. М.</t>
         </is>
       </c>
-      <c r="C30" s="9" t="n"/>
-      <c r="D30" s="11" t="inlineStr">
+      <c r="C36" s="9" t="n"/>
+      <c r="D36" s="11" t="inlineStr">
         <is>
           <t>Сергеев С. А.</t>
         </is>
       </c>
-      <c r="E30" s="9" t="n"/>
-      <c r="F30" s="8" t="inlineStr">
+      <c r="E36" s="9" t="n"/>
+      <c r="F36" s="8" t="inlineStr">
         <is>
           <t>Сергеев С. А.</t>
         </is>
       </c>
-      <c r="G30" s="9" t="n"/>
-    </row>
-    <row r="31" ht="30" customHeight="1">
-      <c r="B31" s="13" t="inlineStr">
+      <c r="G36" s="9" t="n"/>
+    </row>
+    <row r="37" ht="30" customHeight="1">
+      <c r="B37" s="13" t="inlineStr">
         <is>
           <t>2252</t>
         </is>
       </c>
-      <c r="C31" s="9" t="n"/>
-      <c r="D31" s="14" t="inlineStr">
+      <c r="C37" s="9" t="n"/>
+      <c r="D37" s="14" t="inlineStr">
         <is>
           <t>4052</t>
         </is>
       </c>
-      <c r="E31" s="9" t="n"/>
-      <c r="F31" s="12" t="inlineStr">
+      <c r="E37" s="9" t="n"/>
+      <c r="F37" s="12" t="inlineStr">
         <is>
           <t>1252</t>
         </is>
       </c>
-      <c r="G31" s="9" t="n"/>
-    </row>
-    <row r="32">
-      <c r="B32" s="17" t="inlineStr">
-        <is>
-          <t>8 корп. 322 ауд.</t>
-        </is>
-      </c>
-      <c r="C32" s="16" t="n"/>
-      <c r="D32" s="18" t="inlineStr">
-        <is>
-          <t>8 корп. 322 ауд.</t>
-        </is>
-      </c>
-      <c r="E32" s="16" t="n"/>
-      <c r="F32" s="15" t="inlineStr">
-        <is>
-          <t>8 корп. 322 ауд.</t>
-        </is>
-      </c>
-      <c r="G32" s="16" t="n"/>
-    </row>
-    <row r="33">
-      <c r="B33" s="2" t="inlineStr">
+      <c r="G37" s="9" t="n"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="17" t="inlineStr">
+        <is>
+          <t>8 корп. 322 ауд.</t>
+        </is>
+      </c>
+      <c r="C38" s="16" t="n"/>
+      <c r="D38" s="18" t="inlineStr">
+        <is>
+          <t>8 корп. 322 ауд.</t>
+        </is>
+      </c>
+      <c r="E38" s="16" t="n"/>
+      <c r="F38" s="15" t="inlineStr">
+        <is>
+          <t>8 корп. 322 ауд.</t>
+        </is>
+      </c>
+      <c r="G38" s="16" t="n"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="2" t="inlineStr">
         <is>
           <t>ПРАКТИКА</t>
         </is>
       </c>
-      <c r="C33" s="3" t="inlineStr">
+      <c r="C39" s="3" t="inlineStr">
         <is>
           <t>З</t>
         </is>
       </c>
-    </row>
-    <row r="34">
-      <c r="B34" s="8" t="n"/>
-      <c r="C34" s="9" t="n"/>
-    </row>
-    <row r="35" ht="100" customHeight="1">
-      <c r="B35" s="12" t="inlineStr">
+      <c r="F39" s="4" t="inlineStr">
+        <is>
+          <t>ЛЕКЦИЯ</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>Ч/З</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" s="8" t="n"/>
+      <c r="C40" s="9" t="n"/>
+      <c r="F40" s="10" t="n"/>
+      <c r="G40" s="9" t="n"/>
+    </row>
+    <row r="41" ht="100" customHeight="1">
+      <c r="B41" s="12" t="inlineStr">
         <is>
           <t>Молекулярные технологии и электроника</t>
         </is>
       </c>
-      <c r="C35" s="9" t="n"/>
-    </row>
-    <row r="36">
-      <c r="B36" s="8" t="inlineStr">
+      <c r="C41" s="9" t="n"/>
+      <c r="F41" s="13" t="inlineStr">
+        <is>
+          <t>Компьютерные технологии в научных исследованиях</t>
+        </is>
+      </c>
+      <c r="G41" s="9" t="n"/>
+    </row>
+    <row r="42">
+      <c r="B42" s="8" t="inlineStr">
         <is>
           <t>Ушаков Н. М.</t>
         </is>
       </c>
-      <c r="C36" s="9" t="n"/>
-    </row>
-    <row r="37" ht="30" customHeight="1">
-      <c r="B37" s="12" t="inlineStr">
+      <c r="C42" s="9" t="n"/>
+      <c r="F42" s="10" t="inlineStr">
+        <is>
+          <t>Сергеев С. А.</t>
+        </is>
+      </c>
+      <c r="G42" s="9" t="n"/>
+    </row>
+    <row r="43" ht="30" customHeight="1">
+      <c r="B43" s="12" t="inlineStr">
         <is>
           <t>2252</t>
         </is>
       </c>
-      <c r="C37" s="9" t="n"/>
-    </row>
-    <row r="38">
-      <c r="B38" s="15" t="inlineStr">
-        <is>
-          <t>8 корп. 322 ауд.</t>
-        </is>
-      </c>
-      <c r="C38" s="16" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>15:35 - 17:10</t>
-        </is>
-      </c>
-      <c r="B39" s="6" t="inlineStr">
-        <is>
-          <t>ЛАБОРАТОРНАЯ</t>
-        </is>
-      </c>
-      <c r="C39" s="7" t="inlineStr">
-        <is>
-          <t>Ч/З</t>
-        </is>
-      </c>
-      <c r="D39" s="6" t="inlineStr">
-        <is>
-          <t>ЛАБОРАТОРНАЯ</t>
-        </is>
-      </c>
-      <c r="E39" s="7" t="inlineStr">
-        <is>
-          <t>Ч/З</t>
-        </is>
-      </c>
-      <c r="F39" s="6" t="inlineStr">
-        <is>
-          <t>ЛАБОРАТОРНАЯ</t>
-        </is>
-      </c>
-      <c r="G39" s="7" t="inlineStr">
-        <is>
-          <t>Ч/З</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" s="11" t="n"/>
-      <c r="C40" s="9" t="n"/>
-      <c r="D40" s="11" t="n"/>
-      <c r="E40" s="9" t="n"/>
-      <c r="F40" s="11" t="n"/>
-      <c r="G40" s="9" t="n"/>
-    </row>
-    <row r="41" ht="100" customHeight="1">
-      <c r="B41" s="14" t="inlineStr">
-        <is>
-          <t>Основы молекулярной технологии</t>
-        </is>
-      </c>
-      <c r="C41" s="9" t="n"/>
-      <c r="D41" s="14" t="inlineStr">
-        <is>
-          <t>Методы измерений и испытаний полупроводниковых структур электроники</t>
-        </is>
-      </c>
-      <c r="E41" s="9" t="n"/>
-      <c r="F41" s="14" t="inlineStr">
-        <is>
-          <t>Методы и средства измерений, испытаний и контроля при производстве изделий электронной техники</t>
-        </is>
-      </c>
-      <c r="G41" s="9" t="n"/>
-    </row>
-    <row r="42">
-      <c r="B42" s="11" t="inlineStr">
-        <is>
-          <t>Ушаков Н. М.</t>
-        </is>
-      </c>
-      <c r="C42" s="9" t="n"/>
-      <c r="D42" s="11" t="inlineStr">
-        <is>
-          <t>Сергеев С. А.</t>
-        </is>
-      </c>
-      <c r="E42" s="9" t="n"/>
-      <c r="F42" s="11" t="inlineStr">
-        <is>
-          <t>Сергеев С. А.</t>
-        </is>
-      </c>
-      <c r="G42" s="9" t="n"/>
-    </row>
-    <row r="43" ht="30" customHeight="1">
-      <c r="B43" s="14" t="inlineStr">
-        <is>
-          <t>2252</t>
-        </is>
-      </c>
       <c r="C43" s="9" t="n"/>
-      <c r="D43" s="14" t="inlineStr">
-        <is>
-          <t>4052</t>
-        </is>
-      </c>
-      <c r="E43" s="9" t="n"/>
-      <c r="F43" s="14" t="inlineStr">
+      <c r="F43" s="13" t="inlineStr">
         <is>
           <t>1252</t>
         </is>
@@ -1507,19 +1472,13 @@
       <c r="G43" s="9" t="n"/>
     </row>
     <row r="44">
-      <c r="B44" s="18" t="inlineStr">
+      <c r="B44" s="15" t="inlineStr">
         <is>
           <t>8 корп. 322 ауд.</t>
         </is>
       </c>
       <c r="C44" s="16" t="n"/>
-      <c r="D44" s="18" t="inlineStr">
-        <is>
-          <t>8 корп. 322 ауд.</t>
-        </is>
-      </c>
-      <c r="E44" s="16" t="n"/>
-      <c r="F44" s="18" t="inlineStr">
+      <c r="F44" s="17" t="inlineStr">
         <is>
           <t>8 корп. 322 ауд.</t>
         </is>
@@ -1529,65 +1488,142 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
+          <t>15:35 - 17:10</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>ЛАБОРАТОРНАЯ</t>
+        </is>
+      </c>
+      <c r="C45" s="7" t="inlineStr">
+        <is>
+          <t>Ч/З</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>ЛАБОРАТОРНАЯ</t>
+        </is>
+      </c>
+      <c r="E45" s="7" t="inlineStr">
+        <is>
+          <t>Ч/З</t>
+        </is>
+      </c>
+      <c r="F45" s="6" t="inlineStr">
+        <is>
+          <t>ЛАБОРАТОРНАЯ</t>
+        </is>
+      </c>
+      <c r="G45" s="7" t="inlineStr">
+        <is>
+          <t>Ч/З</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" s="11" t="n"/>
+      <c r="C46" s="9" t="n"/>
+      <c r="D46" s="11" t="n"/>
+      <c r="E46" s="9" t="n"/>
+      <c r="F46" s="11" t="n"/>
+      <c r="G46" s="9" t="n"/>
+    </row>
+    <row r="47" ht="100" customHeight="1">
+      <c r="B47" s="14" t="inlineStr">
+        <is>
+          <t>Основы молекулярной технологии</t>
+        </is>
+      </c>
+      <c r="C47" s="9" t="n"/>
+      <c r="D47" s="14" t="inlineStr">
+        <is>
+          <t>Методы измерений и испытаний полупроводниковых структур электроники</t>
+        </is>
+      </c>
+      <c r="E47" s="9" t="n"/>
+      <c r="F47" s="14" t="inlineStr">
+        <is>
+          <t>Методы и средства измерений, испытаний и контроля при производстве изделий электронной техники</t>
+        </is>
+      </c>
+      <c r="G47" s="9" t="n"/>
+    </row>
+    <row r="48">
+      <c r="B48" s="11" t="inlineStr">
+        <is>
+          <t>Ушаков Н. М.</t>
+        </is>
+      </c>
+      <c r="C48" s="9" t="n"/>
+      <c r="D48" s="11" t="inlineStr">
+        <is>
+          <t>Сергеев С. А.</t>
+        </is>
+      </c>
+      <c r="E48" s="9" t="n"/>
+      <c r="F48" s="11" t="inlineStr">
+        <is>
+          <t>Сергеев С. А.</t>
+        </is>
+      </c>
+      <c r="G48" s="9" t="n"/>
+    </row>
+    <row r="49" ht="30" customHeight="1">
+      <c r="B49" s="14" t="inlineStr">
+        <is>
+          <t>2252</t>
+        </is>
+      </c>
+      <c r="C49" s="9" t="n"/>
+      <c r="D49" s="14" t="inlineStr">
+        <is>
+          <t>4052</t>
+        </is>
+      </c>
+      <c r="E49" s="9" t="n"/>
+      <c r="F49" s="14" t="inlineStr">
+        <is>
+          <t>1252</t>
+        </is>
+      </c>
+      <c r="G49" s="9" t="n"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="18" t="inlineStr">
+        <is>
+          <t>8 корп. 322 ауд.</t>
+        </is>
+      </c>
+      <c r="C50" s="16" t="n"/>
+      <c r="D50" s="18" t="inlineStr">
+        <is>
+          <t>8 корп. 322 ауд.</t>
+        </is>
+      </c>
+      <c r="E50" s="16" t="n"/>
+      <c r="F50" s="18" t="inlineStr">
+        <is>
+          <t>8 корп. 322 ауд.</t>
+        </is>
+      </c>
+      <c r="G50" s="16" t="n"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
           <t>17:20 - 18:40</t>
         </is>
       </c>
-      <c r="D45" s="2" t="inlineStr">
+      <c r="D51" s="2" t="inlineStr">
         <is>
           <t>ПРАКТИКА</t>
         </is>
       </c>
-      <c r="E45" s="3" t="inlineStr">
+      <c r="E51" s="3" t="inlineStr">
         <is>
           <t>З</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="D46" s="8" t="n"/>
-      <c r="E46" s="9" t="n"/>
-    </row>
-    <row r="47" ht="100" customHeight="1">
-      <c r="D47" s="12" t="inlineStr">
-        <is>
-          <t>Методы измерений и испытаний полупроводниковых структур электроники</t>
-        </is>
-      </c>
-      <c r="E47" s="9" t="n"/>
-    </row>
-    <row r="48">
-      <c r="D48" s="8" t="inlineStr">
-        <is>
-          <t>Сергеев С. А.</t>
-        </is>
-      </c>
-      <c r="E48" s="9" t="n"/>
-    </row>
-    <row r="49" ht="30" customHeight="1">
-      <c r="D49" s="12" t="inlineStr">
-        <is>
-          <t>4052</t>
-        </is>
-      </c>
-      <c r="E49" s="9" t="n"/>
-    </row>
-    <row r="50">
-      <c r="D50" s="15" t="inlineStr">
-        <is>
-          <t>8 корп. 322 ауд.</t>
-        </is>
-      </c>
-      <c r="E50" s="16" t="n"/>
-    </row>
-    <row r="51">
-      <c r="D51" s="2" t="inlineStr">
-        <is>
-          <t>ПРАКТИКА</t>
-        </is>
-      </c>
-      <c r="E51" s="3" t="inlineStr">
-        <is>
-          <t>Ч</t>
         </is>
       </c>
     </row>
@@ -1598,7 +1634,7 @@
     <row r="53" ht="100" customHeight="1">
       <c r="D53" s="12" t="inlineStr">
         <is>
-          <t>Научно-исследовательская работа</t>
+          <t>Методы измерений и испытаний полупроводниковых структур электроники</t>
         </is>
       </c>
       <c r="E53" s="9" t="n"/>
@@ -1614,7 +1650,7 @@
     <row r="55" ht="30" customHeight="1">
       <c r="D55" s="12" t="inlineStr">
         <is>
-          <t>1252</t>
+          <t>4052</t>
         </is>
       </c>
       <c r="E55" s="9" t="n"/>
@@ -1628,25 +1664,75 @@
       <c r="E56" s="16" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>ПРАКТИКА</t>
+        </is>
+      </c>
+      <c r="E57" s="3" t="inlineStr">
+        <is>
+          <t>Ч</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="D58" s="8" t="n"/>
+      <c r="E58" s="9" t="n"/>
+    </row>
+    <row r="59" ht="100" customHeight="1">
+      <c r="D59" s="12" t="inlineStr">
+        <is>
+          <t>Научно-исследовательская работа</t>
+        </is>
+      </c>
+      <c r="E59" s="9" t="n"/>
+    </row>
+    <row r="60">
+      <c r="D60" s="8" t="inlineStr">
+        <is>
+          <t>Сергеев С. А.</t>
+        </is>
+      </c>
+      <c r="E60" s="9" t="n"/>
+    </row>
+    <row r="61" ht="30" customHeight="1">
+      <c r="D61" s="12" t="inlineStr">
+        <is>
+          <t>1252</t>
+        </is>
+      </c>
+      <c r="E61" s="9" t="n"/>
+    </row>
+    <row r="62">
+      <c r="D62" s="15" t="inlineStr">
+        <is>
+          <t>8 корп. 322 ауд.</t>
+        </is>
+      </c>
+      <c r="E62" s="16" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
         <is>
           <t>18:45 - 20:05</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="143">
+  <mergeCells count="153">
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D60:E60"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="D36:E36"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A45:A50"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D61:E61"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D48:E48"/>
@@ -1656,34 +1742,36 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="J31:K31"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="D56:E56"/>
+    <mergeCell ref="B49:C49"/>
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B32:C32"/>
     <mergeCell ref="J23:K23"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="F34:G34"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="H25:I25"/>
-    <mergeCell ref="F30:G30"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A15:A26"/>
     <mergeCell ref="F42:G42"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
@@ -1691,21 +1779,25 @@
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="F47:G47"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="A15:A32"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F46:G46"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="F28:G28"/>
     <mergeCell ref="A3:A14"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="F48:G48"/>
     <mergeCell ref="L6:M6"/>
-    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="A2"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A33:A44"/>
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J29:K29"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F7:G7"/>
@@ -1714,7 +1806,9 @@
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="F36:G36"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F50:G50"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="J26:K26"/>
@@ -1725,58 +1819,58 @@
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B30:C30"/>
     <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D30:E30"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F49:G49"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B47:C47"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B46:C46"/>
     <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A63"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D40:E40"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="F40:G40"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B48:C48"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:K6"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A45:A56"/>
+    <mergeCell ref="F35:G35"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F38:G38"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A51:A62"/>
+    <mergeCell ref="J32:K32"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D58:E58"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A27:A38"/>
-    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F37:G37"/>
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A57"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B50:C50"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D59:E59"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="H26:I26"/>
   </mergeCells>

</xml_diff>